<commit_message>
Added Update Exercise Functionality
</commit_message>
<xml_diff>
--- a/Documents/Sprint Logs.xlsx
+++ b/Documents/Sprint Logs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT-Digital-Systems-Project\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0BC0F3-3620-47ED-84AC-0AD7D3DC6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{2D0BC0F3-3620-47ED-84AC-0AD7D3DC6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B115CA70-A9FD-4B4C-A987-A300ABC2DD62}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="206">
   <si>
     <t>Location</t>
   </si>
@@ -760,6 +760,36 @@
   <si>
     <t>Completed 80% of Workout History Screen
 Implemented Update Functionality</t>
+  </si>
+  <si>
+    <t>11:30-03:00</t>
+  </si>
+  <si>
+    <t>08:30-12:30</t>
+  </si>
+  <si>
+    <t>Fixed Github Problem
+Implemented Delete Exercise Log Functionality
+Completed 40%  Exercise Log Screen</t>
+  </si>
+  <si>
+    <t>Fix Github problem (Long Paths &amp; Size Limiter)
+Start Exercise Log Screen
+Implement Delete Exercise Log Functionality</t>
+  </si>
+  <si>
+    <t>Complete Exercise Log Screen
+Implement Update Exercise Log Functionality</t>
+  </si>
+  <si>
+    <t>Implemented Exercise Log Screen
+Implemented Update Exercise Log Functionality</t>
+  </si>
+  <si>
+    <t>22:00-01:30</t>
+  </si>
+  <si>
+    <t>13:30-14:10</t>
   </si>
 </sst>
 </file>
@@ -837,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -919,6 +949,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,6 +990,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1224,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2830,7 +2867,7 @@
         <v>191</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="H62" s="9" t="s">
         <v>193</v>
@@ -2856,7 +2893,7 @@
         <v>192</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="H63" s="15" t="s">
         <v>195</v>
@@ -2882,7 +2919,7 @@
         <v>194</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="H64" s="15" t="s">
         <v>197</v>
@@ -2890,9 +2927,11 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="16">
-        <v>45337</v>
-      </c>
-      <c r="B65" s="12"/>
+        <v>45342</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="C65" s="12" t="s">
         <v>15</v>
       </c>
@@ -2902,60 +2941,128 @@
       <c r="E65" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F65" s="19"/>
+      <c r="F65" s="19" t="s">
+        <v>191</v>
+      </c>
       <c r="G65" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="9"/>
+    </row>
+    <row r="66" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>45343</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="G66" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>45344</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G67" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>45345</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
+        <v>45346</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="19"/>
+      <c r="G69" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H65" s="9"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="16"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="9"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A67" s="16"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="19"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A68" s="16"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="9"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A69" s="16"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="24"/>
       <c r="H69" s="9"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
+      <c r="A70" s="16">
+        <v>45347</v>
+      </c>
       <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
+      <c r="C70" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F70" s="19"/>
-      <c r="G70" s="24"/>
+      <c r="G70" s="24" t="s">
+        <v>63</v>
+      </c>
       <c r="H70" s="9"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Allocate Workout Functionality, Fixed Popup Bug, Added Create Workout Screen
</commit_message>
<xml_diff>
--- a/Documents/Sprint Logs.xlsx
+++ b/Documents/Sprint Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{2D0BC0F3-3620-47ED-84AC-0AD7D3DC6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6102E03F-5678-4DF8-B601-3C20E159B910}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{2D0BC0F3-3620-47ED-84AC-0AD7D3DC6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC1B55D-FE5B-4DC9-9E66-1F3434F4F245}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="210">
   <si>
     <t>Location</t>
   </si>
@@ -790,6 +790,24 @@
   </si>
   <si>
     <t>13:30-14:10</t>
+  </si>
+  <si>
+    <t>20:00-00:00</t>
+  </si>
+  <si>
+    <t>Create Allocate Workout Screen
+Implement Delete Workout Functionality
+Implement Update Workout Functionality</t>
+  </si>
+  <si>
+    <t>Created Allocate Workout Screen
+Implemented Delete Workout Functionality
+Implemented Update Workout Functionality</t>
+  </si>
+  <si>
+    <t>Complete Allocate Workout Screen
+Implement Allocate Workout Functionality
+Implement Create Workout Functionality</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3025,11 +3043,13 @@
       </c>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="16">
-        <v>45347</v>
-      </c>
-      <c r="B69" s="12"/>
+        <v>45348</v>
+      </c>
+      <c r="B69" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="C69" s="12" t="s">
         <v>15</v>
       </c>
@@ -3039,84 +3059,156 @@
       <c r="E69" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F69" s="19"/>
+      <c r="F69" s="14" t="s">
+        <v>207</v>
+      </c>
       <c r="G69" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H69" s="9"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="19"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="9"/>
+      <c r="C70" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="19"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="9"/>
-    </row>
-    <row r="72" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="14"/>
+      <c r="G71" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H71" s="14"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="12"/>
       <c r="C72" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>137</v>
+      <c r="D72" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="15" t="s">
-        <v>168</v>
-      </c>
+      <c r="F72" s="14"/>
       <c r="G72" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H72" s="15"/>
+      <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="21"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="H73" s="10"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="21"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="H74" s="10"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H75" s="10"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="14"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H76" s="10"/>
+      <c r="A76" s="16"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="9"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H77" s="10"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H78" s="10"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="9"/>
+    </row>
+    <row r="78" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="16"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H78" s="15"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
       <c r="H79" s="10"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
       <c r="H80" s="10"/>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.3">
@@ -3262,6 +3354,24 @@
     </row>
     <row r="128" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H128" s="10"/>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H129" s="10"/>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H130" s="10"/>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H131" s="10"/>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H132" s="10"/>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H133" s="10"/>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H134" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Added Create Workout and Exercise Screens
</commit_message>
<xml_diff>
--- a/Documents/Sprint Logs.xlsx
+++ b/Documents/Sprint Logs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{2D0BC0F3-3620-47ED-84AC-0AD7D3DC6E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AC1B55D-FE5B-4DC9-9E66-1F3434F4F245}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E130730-A7F5-4015-8470-BFB0A7E6BBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3750" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="216">
   <si>
     <t>Location</t>
   </si>
@@ -808,6 +808,29 @@
     <t>Complete Allocate Workout Screen
 Implement Allocate Workout Functionality
 Implement Create Workout Functionality</t>
+  </si>
+  <si>
+    <t>12:00-16:00</t>
+  </si>
+  <si>
+    <t>23:00-04:00</t>
+  </si>
+  <si>
+    <t>Implement Create Workout Functionality
+Implement Create Exercise Functionality</t>
+  </si>
+  <si>
+    <t>Completed Allocate Workout Screen
+Completed 30% Allocate Workout Functionality
+Completed 5% Create Exercise Funtionality</t>
+  </si>
+  <si>
+    <t>Implemented Create Workout and Create Exercise Functionality</t>
+  </si>
+  <si>
+    <t>Implement Allocate Exercise Functionality
+Implement Update Exercise Functionality
+Implement Delete Exercise Functionality</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1031,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1279,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3070,8 +3089,12 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="16"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="16">
+        <v>45352</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="C70" s="12" t="s">
         <v>15</v>
       </c>
@@ -3085,13 +3108,19 @@
         <v>209</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H70" s="14"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A71" s="16"/>
-      <c r="B71" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="16">
+        <v>45354</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>211</v>
+      </c>
       <c r="C71" s="12" t="s">
         <v>15</v>
       </c>
@@ -3101,14 +3130,20 @@
       <c r="E71" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F71" s="14"/>
+      <c r="F71" s="14" t="s">
+        <v>212</v>
+      </c>
       <c r="G71" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H71" s="14"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A72" s="16"/>
+        <v>9</v>
+      </c>
+      <c r="H71" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="16">
+        <v>45355</v>
+      </c>
       <c r="B72" s="12"/>
       <c r="C72" s="12" t="s">
         <v>15</v>
@@ -3119,14 +3154,18 @@
       <c r="E72" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F72" s="14"/>
+      <c r="F72" s="14" t="s">
+        <v>215</v>
+      </c>
       <c r="G72" s="24" t="s">
         <v>63</v>
       </c>
       <c r="H72" s="14"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A73" s="16"/>
+      <c r="A73" s="16">
+        <v>45356</v>
+      </c>
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
@@ -3136,7 +3175,9 @@
       <c r="H73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="16"/>
+      <c r="A74" s="16">
+        <v>45357</v>
+      </c>
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
@@ -3146,7 +3187,9 @@
       <c r="H74" s="14"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="16"/>
+      <c r="A75" s="16">
+        <v>45358</v>
+      </c>
       <c r="B75" s="12"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>

</xml_diff>

<commit_message>
Implemented Allocate Exercise Allocate Log Screen, Gym Finder Screen, and Exercise Allocate Screen
</commit_message>
<xml_diff>
--- a/Documents/Sprint Logs.xlsx
+++ b/Documents/Sprint Logs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alisu\OneDrive - UWE Bristol\UWE Bristol &amp; Stuff\3rd Year UWE\Digital Systems\Alistana Fitness &amp; Nutrition Tracker\AFNT\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uweacuk-my.sharepoint.com/personal/ali2_suhail_live_uwe_ac_uk/Documents/UWE Bristol &amp; Stuff/3rd Year UWE/Digital Systems/Alistana Fitness &amp; Nutrition Tracker/AFNT/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E130730-A7F5-4015-8470-BFB0A7E6BBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{2E130730-A7F5-4015-8470-BFB0A7E6BBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14D3D21C-BFC0-45F0-8FCB-AC415731D8DA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="224">
   <si>
     <t>Location</t>
   </si>
@@ -831,6 +831,37 @@
     <t>Implement Allocate Exercise Functionality
 Implement Update Exercise Functionality
 Implement Delete Exercise Functionality</t>
+  </si>
+  <si>
+    <t>22:00-02:40</t>
+  </si>
+  <si>
+    <t>Implemented Update and Delete Exercise Functionality
+Completed 50% Allocate Exercise Functionality</t>
+  </si>
+  <si>
+    <t>Implemented Allocate Exercise Log Screen</t>
+  </si>
+  <si>
+    <t>19:00-21:00</t>
+  </si>
+  <si>
+    <t>Implement Allocate Exercise Log Screen
+Fix Bugs in Allocate Exercise Screen</t>
+  </si>
+  <si>
+    <t>Implement Allocate Exercise Functionality
+Create Gym Finder Screen
+Create Allocate Exercise Log Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented Allocate Exercise Log Functionality
+Created Gym Finder Screen
+Created Allocate Exercise Log Screen
+</t>
+  </si>
+  <si>
+    <t>17:00-20:30</t>
   </si>
 </sst>
 </file>
@@ -1031,6 +1062,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1296,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H134"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3142,9 +3177,11 @@
     </row>
     <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="16">
-        <v>45355</v>
-      </c>
-      <c r="B72" s="12"/>
+        <v>45356</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>216</v>
+      </c>
       <c r="C72" s="12" t="s">
         <v>15</v>
       </c>
@@ -3158,54 +3195,102 @@
         <v>215</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H72" s="14"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A73" s="16">
-        <v>45356</v>
-      </c>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="14"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+        <v>45359</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="G73" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="16">
-        <v>45357</v>
-      </c>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="14"/>
+        <v>45360</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="G74" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="16">
-        <v>45358</v>
+        <v>45362</v>
       </c>
       <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="24"/>
-      <c r="H75" s="14"/>
+      <c r="C75" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="19"/>
+      <c r="G75" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H75" s="9"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A76" s="16"/>
+      <c r="A76" s="16">
+        <v>45363</v>
+      </c>
       <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
+      <c r="C76" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="F76" s="19"/>
-      <c r="G76" s="24"/>
+      <c r="G76" s="24" t="s">
+        <v>63</v>
+      </c>
       <c r="H76" s="9"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -3218,88 +3303,102 @@
       <c r="G77" s="24"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="16"/>
       <c r="B78" s="12"/>
-      <c r="C78" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="5" t="s">
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="9"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="16"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="9"/>
+    </row>
+    <row r="80" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="16"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E78" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F78" s="15" t="s">
+      <c r="E80" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="G78" s="24" t="s">
+      <c r="G80" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="H78" s="15"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="21"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="H79" s="10"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A80" s="21"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="H80" s="10"/>
-    </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H80" s="15"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
       <c r="H82" s="10"/>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H83" s="10"/>
     </row>
-    <row r="84" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H84" s="10"/>
     </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H85" s="10"/>
     </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H86" s="10"/>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H87" s="10"/>
     </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H88" s="10"/>
     </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H89" s="10"/>
     </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H90" s="10"/>
     </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H91" s="10"/>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H92" s="10"/>
     </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H93" s="10"/>
     </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H94" s="10"/>
     </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H95" s="10"/>
     </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H96" s="10"/>
     </row>
     <row r="97" spans="8:8" x14ac:dyDescent="0.3">
@@ -3415,6 +3514,12 @@
     </row>
     <row r="134" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H134" s="10"/>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H135" s="10"/>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H136" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>